<commit_message>
Subba Code on 10th Oct abt Phoenix Automation
</commit_message>
<xml_diff>
--- a/SubbaAutomationFramework/TestData/TestData.xlsx
+++ b/SubbaAutomationFramework/TestData/TestData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="15528" windowHeight="3672" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="15384" windowHeight="7452"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
     <sheet name="addUser" sheetId="3" r:id="rId3"/>
+    <sheet name="addCustomer" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P21"/>
+  <oleSize ref="A1:I20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Username</t>
   </si>
@@ -103,13 +104,31 @@
     <t>User Name</t>
   </si>
   <si>
-    <t>John Smith</t>
-  </si>
-  <si>
     <t>subbarao12345</t>
   </si>
   <si>
     <t>jsr12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Smith </t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>Customer Pentacode</t>
+  </si>
+  <si>
+    <t>Customer Code</t>
+  </si>
+  <si>
+    <t>AUTOMATION1</t>
+  </si>
+  <si>
+    <t>AUTOMATION11</t>
+  </si>
+  <si>
+    <t>AUTOMATION111</t>
   </si>
 </sst>
 </file>
@@ -488,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,16 +692,16 @@
     </row>
     <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -690,4 +709,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data added for demo
</commit_message>
<xml_diff>
--- a/SubbaAutomationFramework/TestData/TestData.xlsx
+++ b/SubbaAutomationFramework/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="14016" windowHeight="7452" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="14280" windowHeight="6960" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -122,13 +122,13 @@
     <t>Customer Code</t>
   </si>
   <si>
-    <t>AUTOMATION5</t>
-  </si>
-  <si>
-    <t>AUTOMATION15</t>
-  </si>
-  <si>
-    <t>AUTOMATION115</t>
+    <t>AUTOMATION555</t>
+  </si>
+  <si>
+    <t>AUTOMATION166</t>
+  </si>
+  <si>
+    <t>AUTOMATION11555</t>
   </si>
 </sst>
 </file>
@@ -716,12 +716,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>